<commit_message>
v 25.02.04 Updates for Science test file and setting override to show accommodations for all students.
</commit_message>
<xml_diff>
--- a/Science MSU Data Dictionary.xlsx
+++ b/Science MSU Data Dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Repos\AKPSUG-Accom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D40C628-B571-4DD4-A50F-7E7F31E85126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{177B5CFC-38F2-4B57-8890-61D7ABD4907C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32450" yWindow="2910" windowWidth="29840" windowHeight="15460" xr2:uid="{738CAF26-924C-4743-B4B5-7BBD7404522E}"/>
+    <workbookView xWindow="560" yWindow="5960" windowWidth="23430" windowHeight="12560" xr2:uid="{738CAF26-924C-4743-B4B5-7BBD7404522E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="71">
   <si>
     <t>District Code</t>
   </si>
@@ -87,9 +87,6 @@
     <t>Grade</t>
   </si>
   <si>
-    <t>Race/Ethnicity</t>
-  </si>
-  <si>
     <t>Disability Status</t>
   </si>
   <si>
@@ -106,9 +103,6 @@
   </si>
   <si>
     <t>Parent/Guardian on Active Duty Military Status</t>
-  </si>
-  <si>
-    <t>[S_AK_STU_X]Suffix</t>
   </si>
   <si>
     <t>[Students]DOB</t>
@@ -149,9 +143,6 @@
     <t>[S_AK_STU_X]Disability_Code</t>
   </si>
   <si>
-    <t>If the code is 01-14 a 'Y' will be displayed. Otherwise it will be a 'N'</t>
-  </si>
-  <si>
     <t>[S_AK_STU_X]Section504</t>
   </si>
   <si>
@@ -164,12 +155,6 @@
     <t>[S_AK_STU_X]ActiveDuty_PG</t>
   </si>
   <si>
-    <t>Science - Text-To-Speech (Not Including ELA Reading Passages)</t>
-  </si>
-  <si>
-    <t>Science - Student provided non-embedded accommodation(s) as noted in IEP or 504 plan.</t>
-  </si>
-  <si>
     <t>Note</t>
   </si>
   <si>
@@ -200,25 +185,93 @@
     <t>[S_AK_STU_X]Econ</t>
   </si>
   <si>
-    <t>[U_AKPSUG_AKTEST]SC_TTS</t>
-  </si>
-  <si>
-    <t>[U_AKPSUG_AKTEST]SC_NON_EMBED</t>
-  </si>
-  <si>
-    <t>[U_AKPSUG_AKTEST]SC_POD</t>
-  </si>
-  <si>
-    <t>Science - Print on Demand</t>
-  </si>
-  <si>
     <t>Report Header2</t>
   </si>
   <si>
     <t>#</t>
   </si>
   <si>
-    <t>The report will show a Y if the checkbox on the Alaska State Administration page is checked (the actual data is either 1 or null)</t>
+    <t>[STUDENTCOREFIELDS]pscore_legal_suffix or [S_AK_STU_X]Suffix</t>
+  </si>
+  <si>
+    <t>Ethnicity -
+Hispanic/Latino</t>
+  </si>
+  <si>
+    <t>[Students]FedEthnicity</t>
+  </si>
+  <si>
+    <t>Y', otherwise blank</t>
+  </si>
+  <si>
+    <t>If the legal suffix field is used it will use that value, otherwise it will use the regular suffix field.</t>
+  </si>
+  <si>
+    <t>Race - American Indian/Alaskan Native</t>
+  </si>
+  <si>
+    <t>Not Used</t>
+  </si>
+  <si>
+    <t>Race - Asian</t>
+  </si>
+  <si>
+    <t>Race - Black/African American</t>
+  </si>
+  <si>
+    <t>Race - Pacific
+Islander/Hawaiian</t>
+  </si>
+  <si>
+    <t>Race - White</t>
+  </si>
+  <si>
+    <t>Alaska Districts use column 28 for race code.</t>
+  </si>
+  <si>
+    <t>IEP Status</t>
+  </si>
+  <si>
+    <t>[S_AK_STU_X]Disability Code</t>
+  </si>
+  <si>
+    <t>If student does not have a value in [S_AK_STU_X]transfer_ge_date, or the date is in the future, and has a disability code this is element will show the student disability code without a leading 0.</t>
+  </si>
+  <si>
+    <t>If student does not have a value in [S_AK_STU_X]transfer_ge_date, or the date is in the future, and has a disability code this is element will resolve in a  'Y'.</t>
+  </si>
+  <si>
+    <t>Science Accommodations</t>
+  </si>
+  <si>
+    <t>[U_AKPSUG_AKTEST]SC_TTS or [U_AKPSUG_AKTEST]POD and [U_AKPSUG_AKTEST]SC_TTS</t>
+  </si>
+  <si>
+    <t>This will resolve to a pipe (|) delimited list of accommodations. Students can have either TTS|SPN, POD|SPN or POD as students cannot have POD and TTS.</t>
+  </si>
+  <si>
+    <t>Special Circumstances</t>
+  </si>
+  <si>
+    <t>[U_AKPSUG_AKTEST]SC_NOT_TESTED</t>
+  </si>
+  <si>
+    <t>Special Circumstance Code for eligible students not taking the Science Test</t>
+  </si>
+  <si>
+    <t>Registration Name</t>
+  </si>
+  <si>
+    <t>[U_AKPSUG_AKTEST]SC_GROUP</t>
+  </si>
+  <si>
+    <t>The Science - Test Group Name entered on the student accommodation page.</t>
+  </si>
+  <si>
+    <t>State Defined Optional Data</t>
+  </si>
+  <si>
+    <t>State Defined student race code (Replaces fields 13-17)</t>
   </si>
 </sst>
 </file>
@@ -269,15 +322,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -301,8 +351,8 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -400,8 +450,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7950601A-D55A-408B-AACA-62334041F2E4}" name="Table1" displayName="Table1" ref="A1:D22" totalsRowShown="0">
-  <autoFilter ref="A1:D22" xr:uid="{CCE2467A-F933-40C7-99A1-3B246FB54958}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7950601A-D55A-408B-AACA-62334041F2E4}" name="Table1" displayName="Table1" ref="A1:D29" totalsRowShown="0">
+  <autoFilter ref="A1:D29" xr:uid="{CCE2467A-F933-40C7-99A1-3B246FB54958}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -418,9 +468,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -458,7 +508,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -564,7 +614,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -706,7 +756,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -714,321 +764,417 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7511A7ED-2D6F-4294-AFFE-C363D701DA2B}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A4" zoomScale="145" zoomScaleNormal="100" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="145" zoomScaleNormal="100" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.36328125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="2.36328125" style="7" customWidth="1"/>
     <col min="2" max="2" width="19.6328125" style="2" customWidth="1"/>
     <col min="3" max="3" width="25.26953125" style="2" customWidth="1"/>
     <col min="4" max="4" width="42.36328125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
-        <v>52</v>
+      <c r="A1" s="7" t="s">
+        <v>43</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="22" x14ac:dyDescent="0.35">
+      <c r="A2" s="8">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="22" x14ac:dyDescent="0.35">
+      <c r="A3" s="8">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="8">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="9">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="22" x14ac:dyDescent="0.35">
+      <c r="A6" s="9">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="22" x14ac:dyDescent="0.35">
+      <c r="A7" s="9">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="22" x14ac:dyDescent="0.35">
+      <c r="A8" s="9">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="22" x14ac:dyDescent="0.35">
-      <c r="A2" s="9">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="D8" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="22" x14ac:dyDescent="0.35">
+      <c r="A9" s="9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="22" x14ac:dyDescent="0.35">
+      <c r="A10" s="9">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="9">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="9">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:4" ht="22" x14ac:dyDescent="0.35">
+      <c r="A13" s="9">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="22" x14ac:dyDescent="0.35">
+      <c r="A14" s="9">
+        <v>13</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="9">
+        <v>14</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="9">
+        <v>15</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="22" x14ac:dyDescent="0.35">
+      <c r="A17" s="9">
+        <v>16</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="9">
+        <v>17</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="32.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="9">
+        <v>18</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="22" x14ac:dyDescent="0.35">
-      <c r="A3" s="9">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="9">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="10">
-        <v>4</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="22" x14ac:dyDescent="0.35">
-      <c r="A6" s="10">
-        <v>5</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="22" x14ac:dyDescent="0.35">
-      <c r="A7" s="10">
-        <v>6</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="5" t="s">
+      <c r="D19" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="9">
+        <v>19</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="1:4" ht="32.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="9">
+        <v>20</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" s="9">
+        <v>21</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="1:4" ht="22" x14ac:dyDescent="0.35">
+      <c r="A23" s="9">
+        <v>22</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="22" x14ac:dyDescent="0.35">
-      <c r="A8" s="10">
-        <v>7</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="10">
-        <v>8</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="5" t="s">
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" s="9">
+        <v>23</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="1:4" ht="22" x14ac:dyDescent="0.35">
+      <c r="A25" s="9">
         <v>24</v>
       </c>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="1:4" ht="22" x14ac:dyDescent="0.35">
-      <c r="A10" s="10">
-        <v>9</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="10">
-        <v>10</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="5" t="s">
+      <c r="B25" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="1:4" ht="35" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="9">
         <v>25</v>
       </c>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="10">
-        <v>11</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="5" t="s">
+      <c r="B26" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="9">
         <v>26</v>
       </c>
-      <c r="D12" s="4"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="10">
-        <v>12</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="5" t="s">
+      <c r="B27" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="22" x14ac:dyDescent="0.35">
+      <c r="A28" s="9">
+        <v>27</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" s="9">
         <v>28</v>
       </c>
-      <c r="D13" s="4"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="10">
-        <v>13</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="10">
-        <v>14</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="4"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="10">
-        <v>15</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="4"/>
-    </row>
-    <row r="17" spans="1:4" ht="22" x14ac:dyDescent="0.35">
-      <c r="A17" s="10">
-        <v>16</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="10">
-        <v>17</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="1:4" ht="22" x14ac:dyDescent="0.35">
-      <c r="A19" s="10">
-        <v>18</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="1:4" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="10">
-        <v>19</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="10">
-        <v>20</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="22" x14ac:dyDescent="0.35">
-      <c r="A22" s="10">
-        <v>21</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" s="11"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="4"/>
+      <c r="B29" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>70</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>
-    <oddHeader xml:space="preserve">&amp;CAKPSUG State Test Accommodations Plugin (v22.02.25) 
+    <oddHeader xml:space="preserve">&amp;CAKPSUG State Test Accommodations Plugin (v25.02.04) 
 Science MSU File Data Dictionary </oddHeader>
   </headerFooter>
   <tableParts count="1">

</xml_diff>